<commit_message>
Archivo re correlativas completo con plan sistemas 2024/2025
</commit_message>
<xml_diff>
--- a/ETL/data/materias.xlsx
+++ b/ETL/data/materias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\asistente-virtual-unla\ETL\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DA2D06-E405-4AEA-A34A-C4A7FBD6442B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FF6A18-6E79-44AD-B898-B9D091F242BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="79">
   <si>
     <t>Carrera</t>
   </si>
@@ -234,10 +234,34 @@
     <t>Seminario Optativo*</t>
   </si>
   <si>
-    <t>["Matematica Discreta","Análisis matematico I"]</t>
-  </si>
-  <si>
-    <t>[""]</t>
+    <t>["Matematica Discreta","Analisis matematico I"]</t>
+  </si>
+  <si>
+    <t>Escenarios Tecnologicos </t>
+  </si>
+  <si>
+    <t>Aspectos sociales y profesionales de la Informatica</t>
+  </si>
+  <si>
+    <t>Practicas Preprofesionales II</t>
+  </si>
+  <si>
+    <t>Taller de Proyectos I+D+i</t>
+  </si>
+  <si>
+    <t>["Proyecto de Software","Taller de Metodologia de la Investigacion","Probabilidad y Estadistica"]</t>
+  </si>
+  <si>
+    <t>["Practicas Pre-profesionales I"]</t>
+  </si>
+  <si>
+    <t>["Sistemas y Organizaciones"]</t>
+  </si>
+  <si>
+    <t>["Ingenieria de Software II","Bases de Datos I","Redes y Comunicaciones","Orientacion a Objetos II","Sistemas Operativos"]</t>
+  </si>
+  <si>
+    <t>Espacios de integración</t>
   </si>
 </sst>
 </file>
@@ -562,14 +586,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="13.77734375" customWidth="1"/>
     <col min="3" max="3" width="31.44140625" customWidth="1"/>
     <col min="4" max="4" width="37.77734375" customWidth="1"/>
     <col min="5" max="5" width="18.44140625" customWidth="1"/>
@@ -1070,6 +1095,15 @@
       <c r="E20">
         <v>6</v>
       </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>96</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
@@ -1087,6 +1121,15 @@
       <c r="E21">
         <v>6</v>
       </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>96</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -1104,6 +1147,15 @@
       <c r="E22">
         <v>6</v>
       </c>
+      <c r="F22">
+        <v>6</v>
+      </c>
+      <c r="G22">
+        <v>96</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -1118,6 +1170,15 @@
       <c r="E23">
         <v>6</v>
       </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>64</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -1132,6 +1193,12 @@
       <c r="E24">
         <v>6</v>
       </c>
+      <c r="G24">
+        <v>80</v>
+      </c>
+      <c r="H24" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -1149,6 +1216,15 @@
       <c r="E25">
         <v>7</v>
       </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>64</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -1166,6 +1242,15 @@
       <c r="E26">
         <v>7</v>
       </c>
+      <c r="F26">
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>64</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -1183,6 +1268,15 @@
       <c r="E27">
         <v>7</v>
       </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>96</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -1200,6 +1294,15 @@
       <c r="E28">
         <v>7</v>
       </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>96</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -1217,6 +1320,15 @@
       <c r="E29">
         <v>7</v>
       </c>
+      <c r="F29">
+        <v>6</v>
+      </c>
+      <c r="G29">
+        <v>96</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -1234,6 +1346,15 @@
       <c r="E30">
         <v>8</v>
       </c>
+      <c r="F30">
+        <v>6</v>
+      </c>
+      <c r="G30">
+        <v>96</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -1251,6 +1372,15 @@
       <c r="E31">
         <v>8</v>
       </c>
+      <c r="F31">
+        <v>6</v>
+      </c>
+      <c r="G31">
+        <v>96</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -1268,8 +1398,17 @@
       <c r="E32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32">
+        <v>6</v>
+      </c>
+      <c r="G32">
+        <v>96</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1282,8 +1421,17 @@
       <c r="E33">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>96</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1296,8 +1444,17 @@
       <c r="E34">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34">
+        <v>6</v>
+      </c>
+      <c r="G34">
+        <v>96</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1308,13 +1465,22 @@
         <v>66</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="E35">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35">
+        <v>6</v>
+      </c>
+      <c r="G35">
+        <v>96</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1330,8 +1496,17 @@
       <c r="E36">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36">
+        <v>6</v>
+      </c>
+      <c r="G36">
+        <v>96</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1344,8 +1519,113 @@
       <c r="E37">
         <v>9</v>
       </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>2024</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38">
+        <v>10</v>
+      </c>
+      <c r="F38">
+        <v>4</v>
+      </c>
+      <c r="G38">
+        <v>64</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <v>2024</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39">
+        <v>10</v>
+      </c>
+      <c r="F39">
+        <v>4</v>
+      </c>
+      <c r="G39">
+        <v>64</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>2024</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" t="s">
+        <v>75</v>
+      </c>
+      <c r="E40">
+        <v>10</v>
+      </c>
+      <c r="G40">
+        <v>7</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <v>2024</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41">
+        <v>10</v>
+      </c>
+      <c r="F41">
+        <v>6</v>
+      </c>
+      <c r="G41">
+        <v>64</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>